<commit_message>
Unit test cases  for CRM
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmgupt1\Documents\UiPath\RpaUiPathProcess\Processes\IAA_VevoCheck_1.0\IAA_VevoCheck\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmgupt1\Documents\UiPath\RpaUiPathProcess\Processes\IAA_VevoCheck\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4406,7 +4406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes for send email and process transaction
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -177,9 +177,6 @@
     <t>SSO_rpa00001</t>
   </si>
   <si>
-    <t>Vevo_ImmiAccount</t>
-  </si>
-  <si>
     <t>Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential)</t>
   </si>
   <si>
@@ -195,280 +192,238 @@
     <t>TBC</t>
   </si>
   <si>
+    <t>https://online.immi.gov.au/lusc/login</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM  URL for Dev environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM  URL for Test environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM URL for Staging environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM URL for Prod environment</t>
+  </si>
+  <si>
+    <t>Immi Account login URL for Vevo Check, external website</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_DEV</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to DEV environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_TEST</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to TEST environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_STAGING</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to STAGING environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_PROD</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to PROD environment</t>
+  </si>
+  <si>
+    <t>manish.gupta@uq.edu.au</t>
+  </si>
+  <si>
+    <t>IAA_VevoCheck</t>
+  </si>
+  <si>
+    <t>IAA_VevoCheck-1.0</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number field label incorrect or missing - should be "Passport Number:"</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth field label incorrect or missing - should be "Date of Birth:".</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth in incorrect format - should be dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document field label incorrect or missing - should be "Country of Document:"</t>
+  </si>
+  <si>
+    <t>VevoFileNamePrefix</t>
+  </si>
+  <si>
+    <t>VevoFileNamePattern</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check*</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check_</t>
+  </si>
+  <si>
+    <t>DownloadLocation</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Downloads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
+  </si>
+  <si>
+    <t>File name pattern for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>File path for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>Config Not Initialised</t>
+  </si>
+  <si>
+    <t>Mode Asset Missing</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL_</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL</t>
+  </si>
+  <si>
+    <t>Credentials_ImmiAccount</t>
+  </si>
+  <si>
+    <t>Credentials_CRM</t>
+  </si>
+  <si>
+    <t>International RPA Vevo Check</t>
+  </si>
+  <si>
+    <t>OracleCRM_TabHeader</t>
+  </si>
+  <si>
+    <t>Vevo Check Out</t>
+  </si>
+  <si>
+    <t>OracleCRM_VevoCheckOut</t>
+  </si>
+  <si>
+    <t>Deafult dashboard tab header name</t>
+  </si>
+  <si>
+    <t>IAS Category name for Vevo Check Out queue</t>
+  </si>
+  <si>
+    <t>C:\Users\uqmgupt1\Downloads</t>
+  </si>
+  <si>
+    <t>FN_Label_Missing</t>
+  </si>
+  <si>
+    <t>FN_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_IncorrectFormat</t>
+  </si>
+  <si>
+    <t>PN_Value_Missing</t>
+  </si>
+  <si>
+    <t>PN_Label_Missing</t>
+  </si>
+  <si>
+    <t>CoD_Label_Missing</t>
+  </si>
+  <si>
+    <t>CoD_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_Label_Missing</t>
+  </si>
+  <si>
+    <t>Couldn't find my operation mode asset at OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>Couldn't get my settings from the config: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An unexpected error occurred in CRM: </t>
+  </si>
+  <si>
+    <t>SystemException_Immi</t>
+  </si>
+  <si>
+    <t>SystemException_CRM</t>
+  </si>
+  <si>
+    <t>ImmiErrorVevoInput</t>
+  </si>
+  <si>
+    <t>An exception occurred while entering Vevo details on Immi website</t>
+  </si>
+  <si>
+    <t>ImmiErrorDownloadSearchResult</t>
+  </si>
+  <si>
+    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
+  </si>
+  <si>
+    <t>smtpServer</t>
+  </si>
+  <si>
+    <t>smtp.uq.edu.au</t>
+  </si>
+  <si>
+    <t>smtpPort</t>
+  </si>
+  <si>
+    <t>rpa.ads@its.uq.edu.au</t>
+  </si>
+  <si>
+    <t>IAA_Vevo_ImmiAccount</t>
+  </si>
+  <si>
+    <t>IAA_Vevo_BusinessNotificationList</t>
+  </si>
+  <si>
+    <t>Text_BusinessNotificationList</t>
+  </si>
+  <si>
+    <t>Business users distribution list to be notified in case of application error during Sign In process</t>
+  </si>
+  <si>
+    <t>EmailSenderName</t>
+  </si>
+  <si>
+    <t>EmailFrom</t>
+  </si>
+  <si>
     <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
-  </si>
-  <si>
-    <t>https://online.immi.gov.au/lusc/login</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM  URL for Dev environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM  URL for Test environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM URL for Staging environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM URL for Prod environment</t>
-  </si>
-  <si>
-    <t>Immi Account login URL for Vevo Check, external website</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_DEV</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to DEV environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_TEST</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to TEST environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_STAGING</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to STAGING environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_PROD</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to PROD environment</t>
-  </si>
-  <si>
-    <t>manish.gupta@uq.edu.au</t>
-  </si>
-  <si>
-    <t>IAA_VevoCheck</t>
-  </si>
-  <si>
-    <t>IAA_VevoCheck-1.0</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number field label incorrect or missing - should be "Passport Number:"</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth field label incorrect or missing - should be "Date of Birth:".</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth in incorrect format - should be dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document field label incorrect or missing - should be "Country of Document:"</t>
-  </si>
-  <si>
-    <t>VevoFileNamePrefix</t>
-  </si>
-  <si>
-    <t>VevoFileNamePattern</t>
-  </si>
-  <si>
-    <t>VEVO Visa Details Check*</t>
-  </si>
-  <si>
-    <t>VEVO Visa Details Check_</t>
-  </si>
-  <si>
-    <t>DownloadLocation</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Downloads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
-  </si>
-  <si>
-    <t>File name pattern for all document retrived from Immi website</t>
-  </si>
-  <si>
-    <t>File path for all document retrived from Immi website</t>
-  </si>
-  <si>
-    <t>Config Not Initialised</t>
-  </si>
-  <si>
-    <t>Mode Asset Missing</t>
-  </si>
-  <si>
-    <t>Extras</t>
-  </si>
-  <si>
-    <t>RuleException_NoTicketsToProcess</t>
-  </si>
-  <si>
-    <t>OracleCRM_URL_</t>
-  </si>
-  <si>
-    <t>OracleCRM_URL</t>
-  </si>
-  <si>
-    <t>Credentials_ImmiAccount</t>
-  </si>
-  <si>
-    <t>Credentials_CRM</t>
-  </si>
-  <si>
-    <t>International RPA Vevo Check</t>
-  </si>
-  <si>
-    <t>OracleCRM_TabHeader</t>
-  </si>
-  <si>
-    <t>Vevo Check Out</t>
-  </si>
-  <si>
-    <t>OracleCRM_VevoCheckOut</t>
-  </si>
-  <si>
-    <t>Deafult dashboard tab header name</t>
-  </si>
-  <si>
-    <t>IAS Category name for Vevo Check Out queue</t>
-  </si>
-  <si>
-    <t>C:\Users\uqmgupt1\Downloads</t>
-  </si>
-  <si>
-    <t>FN_Label_Missing</t>
-  </si>
-  <si>
-    <t>FN_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_IncorrectFormat</t>
-  </si>
-  <si>
-    <t>PN_Value_Missing</t>
-  </si>
-  <si>
-    <t>PN_Label_Missing</t>
-  </si>
-  <si>
-    <t>CoD_Label_Missing</t>
-  </si>
-  <si>
-    <t>CoD_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_Label_Missing</t>
-  </si>
-  <si>
-    <t>No CRM Ticket</t>
-  </si>
-  <si>
-    <t>RuleException_FamilyName</t>
-  </si>
-  <si>
-    <t>Family Name field label</t>
-  </si>
-  <si>
-    <t>Family Name field value</t>
-  </si>
-  <si>
-    <t>RuleException_DateOfBirth</t>
-  </si>
-  <si>
-    <t>RuleException_Passport_Number</t>
-  </si>
-  <si>
-    <t>RuleException_CountryOfDocument</t>
-  </si>
-  <si>
-    <t>Date of Birth field label</t>
-  </si>
-  <si>
-    <t>Date of Birth field value</t>
-  </si>
-  <si>
-    <t>Passport Number field label</t>
-  </si>
-  <si>
-    <t>Passport Number field value</t>
-  </si>
-  <si>
-    <t>Country of Document field label</t>
-  </si>
-  <si>
-    <t>Couldn't find my operation mode asset at OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>Couldn't get my settings from the config: {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Family Name field label for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Family Name field value for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Date of Birth field label for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Date of Birth field value for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Passport Number field label for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Passport Number field value for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Country of Document field label for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find Country of Document field value for Case Reference {0}</t>
-  </si>
-  <si>
-    <t>Couldn't find any pending CRM ticket in Vevo Check In category</t>
-  </si>
-  <si>
-    <t>RuleException_InvalidData</t>
-  </si>
-  <si>
-    <t>1.5: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An unexpected error occurred in CRM: </t>
-  </si>
-  <si>
-    <t>SystemException_Immi</t>
-  </si>
-  <si>
-    <t>SystemException_CRM</t>
-  </si>
-  <si>
-    <t>ImmiErrorVevoInput</t>
-  </si>
-  <si>
-    <t>An exception occurred while entering Vevo details on Immi website</t>
-  </si>
-  <si>
-    <t>ImmiErrorDownloadSearchResult</t>
-  </si>
-  <si>
-    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
   </si>
 </sst>
 </file>
@@ -541,11 +496,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,7 +835,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -892,7 +847,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
@@ -904,10 +859,10 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -915,10 +870,10 @@
         <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,10 +881,10 @@
         <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -937,85 +892,99 @@
         <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="9">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1989,6 +1958,8 @@
     <hyperlink ref="B13" r:id="rId4"/>
     <hyperlink ref="B14" r:id="rId5"/>
     <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B16" r:id="rId7"/>
+    <hyperlink ref="B15" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1998,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2067,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2228,149 +2199,94 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
         <v>102</v>
-      </c>
-      <c r="B43" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3335,7 +3251,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3381,27 +3297,37 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4404,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4426,29 +4352,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>115</v>
+      </c>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -4456,178 +4382,114 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>139</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>131</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>133</v>
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>134</v>
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>135</v>
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>136</v>
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>137</v>
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>138</v>
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="7"/>
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>141</v>
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Changes for screenshot capture and exceptions
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -17,12 +17,12 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Messages" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -174,256 +174,259 @@
     <t>OracleCRM_URL_PROD</t>
   </si>
   <si>
+    <t>ImmiPortal_URL</t>
+  </si>
+  <si>
+    <t>https://uqapplications.crm.test.uq.edu.au/AgentWeb/</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM  URL for Dev environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM  URL for Test environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM URL for Staging environment</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM URL for Prod environment</t>
+  </si>
+  <si>
+    <t>Immi Account login URL for Vevo Check, external website</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_DEV</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to DEV environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_TEST</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to TEST environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_STAGING</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to STAGING environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_PROD</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to PROD environment</t>
+  </si>
+  <si>
+    <t>manish.gupta@uq.edu.au</t>
+  </si>
+  <si>
+    <t>IAA_VevoCheck</t>
+  </si>
+  <si>
+    <t>IAA_VevoCheck-1.0</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number field label incorrect or missing - should be "Passport Number:"</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth field label incorrect or missing - should be "Date of Birth:".</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth in incorrect format - should be dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document value is missing.</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document field label incorrect or missing - should be "Country of Document:"</t>
+  </si>
+  <si>
+    <t>VevoFileNamePrefix</t>
+  </si>
+  <si>
+    <t>VevoFileNamePattern</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check*</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check_</t>
+  </si>
+  <si>
+    <t>DownloadLocation</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Downloads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
+  </si>
+  <si>
+    <t>File name pattern for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>File path for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>Config Not Initialised</t>
+  </si>
+  <si>
+    <t>Mode Asset Missing</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL_</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL</t>
+  </si>
+  <si>
+    <t>Credentials_ImmiAccount</t>
+  </si>
+  <si>
+    <t>Credentials_CRM</t>
+  </si>
+  <si>
+    <t>International RPA Vevo Check</t>
+  </si>
+  <si>
+    <t>Vevo Check Out</t>
+  </si>
+  <si>
+    <t>IAS Category name for Vevo Check Out queue</t>
+  </si>
+  <si>
+    <t>FN_Label_Missing</t>
+  </si>
+  <si>
+    <t>FN_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_IncorrectFormat</t>
+  </si>
+  <si>
+    <t>PN_Value_Missing</t>
+  </si>
+  <si>
+    <t>PN_Label_Missing</t>
+  </si>
+  <si>
+    <t>CoD_Label_Missing</t>
+  </si>
+  <si>
+    <t>CoD_Value_Missing</t>
+  </si>
+  <si>
+    <t>DoB_Label_Missing</t>
+  </si>
+  <si>
+    <t>Couldn't find my operation mode asset at OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>Couldn't get my settings from the config: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An unexpected error occurred in CRM: </t>
+  </si>
+  <si>
+    <t>SystemException_Immi</t>
+  </si>
+  <si>
+    <t>SystemException_CRM</t>
+  </si>
+  <si>
+    <t>ImmiErrorVevoInput</t>
+  </si>
+  <si>
+    <t>An exception occurred while entering Vevo details on Immi website</t>
+  </si>
+  <si>
+    <t>ImmiErrorDownloadSearchResult</t>
+  </si>
+  <si>
+    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
+  </si>
+  <si>
+    <t>smtpServer</t>
+  </si>
+  <si>
+    <t>smtp.uq.edu.au</t>
+  </si>
+  <si>
+    <t>smtpPort</t>
+  </si>
+  <si>
+    <t>rpa.ads@its.uq.edu.au</t>
+  </si>
+  <si>
+    <t>EmailSenderName</t>
+  </si>
+  <si>
+    <t>EmailFrom</t>
+  </si>
+  <si>
+    <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
+  </si>
+  <si>
+    <t>Victor's (RPA bot for Vevo check) Immi account login  (Type: Credential)</t>
+  </si>
+  <si>
+    <t>VevoDisplayName</t>
+  </si>
+  <si>
+    <t>VevoDashboardName</t>
+  </si>
+  <si>
+    <t>RPA Vevo Check</t>
+  </si>
+  <si>
+    <t>VevoCheckOutCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deafult dashboard tab header name in Oracle CRM </t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>RPA robot display name in Oracle CRM</t>
+  </si>
+  <si>
+    <t>https://online.immi.gov.au/lusc/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
+  </si>
+  <si>
     <t>SSO_rpa00001</t>
   </si>
   <si>
-    <t>Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential)</t>
-  </si>
-  <si>
-    <t>Victor's (RPA bot for Vevo check) Immi account login  (Type: Credential)</t>
-  </si>
-  <si>
-    <t>ImmiPortal_URL</t>
-  </si>
-  <si>
-    <t>https://uqapplications.crm.test.uq.edu.au/AgentWeb/</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>https://online.immi.gov.au/lusc/login</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM  URL for Dev environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM  URL for Test environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM URL for Staging environment</t>
-  </si>
-  <si>
-    <t>UQ Oracle CRM URL for Prod environment</t>
-  </si>
-  <si>
-    <t>Immi Account login URL for Vevo Check, external website</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_DEV</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to DEV environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_TEST</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to TEST environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_STAGING</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to STAGING environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_PROD</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to PROD environment</t>
-  </si>
-  <si>
-    <t>manish.gupta@uq.edu.au</t>
-  </si>
-  <si>
-    <t>IAA_VevoCheck</t>
-  </si>
-  <si>
-    <t>IAA_VevoCheck-1.0</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number field label incorrect or missing - should be "Passport Number:"</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth field label incorrect or missing - should be "Date of Birth:".</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth in incorrect format - should be dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Passport Number value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document value is missing.</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document field label incorrect or missing - should be "Country of Document:"</t>
-  </si>
-  <si>
-    <t>VevoFileNamePrefix</t>
-  </si>
-  <si>
-    <t>VevoFileNamePattern</t>
-  </si>
-  <si>
-    <t>VEVO Visa Details Check*</t>
-  </si>
-  <si>
-    <t>VEVO Visa Details Check_</t>
-  </si>
-  <si>
-    <t>DownloadLocation</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Downloads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
-  </si>
-  <si>
-    <t>File name pattern for all document retrived from Immi website</t>
-  </si>
-  <si>
-    <t>File path for all document retrived from Immi website</t>
-  </si>
-  <si>
-    <t>Config Not Initialised</t>
-  </si>
-  <si>
-    <t>Mode Asset Missing</t>
-  </si>
-  <si>
-    <t>Extras</t>
-  </si>
-  <si>
-    <t>OracleCRM_URL_</t>
-  </si>
-  <si>
-    <t>OracleCRM_URL</t>
-  </si>
-  <si>
-    <t>Credentials_ImmiAccount</t>
-  </si>
-  <si>
-    <t>Credentials_CRM</t>
-  </si>
-  <si>
-    <t>International RPA Vevo Check</t>
-  </si>
-  <si>
-    <t>OracleCRM_TabHeader</t>
-  </si>
-  <si>
-    <t>Vevo Check Out</t>
-  </si>
-  <si>
-    <t>OracleCRM_VevoCheckOut</t>
-  </si>
-  <si>
-    <t>Deafult dashboard tab header name</t>
-  </si>
-  <si>
-    <t>IAS Category name for Vevo Check Out queue</t>
-  </si>
-  <si>
-    <t>C:\Users\uqmgupt1\Downloads</t>
-  </si>
-  <si>
-    <t>FN_Label_Missing</t>
-  </si>
-  <si>
-    <t>FN_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_IncorrectFormat</t>
-  </si>
-  <si>
-    <t>PN_Value_Missing</t>
-  </si>
-  <si>
-    <t>PN_Label_Missing</t>
-  </si>
-  <si>
-    <t>CoD_Label_Missing</t>
-  </si>
-  <si>
-    <t>CoD_Value_Missing</t>
-  </si>
-  <si>
-    <t>DoB_Label_Missing</t>
-  </si>
-  <si>
-    <t>Couldn't find my operation mode asset at OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>Couldn't get my settings from the config: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An unexpected error occurred in CRM: </t>
-  </si>
-  <si>
-    <t>SystemException_Immi</t>
-  </si>
-  <si>
-    <t>SystemException_CRM</t>
-  </si>
-  <si>
-    <t>ImmiErrorVevoInput</t>
-  </si>
-  <si>
-    <t>An exception occurred while entering Vevo details on Immi website</t>
-  </si>
-  <si>
-    <t>ImmiErrorDownloadSearchResult</t>
-  </si>
-  <si>
-    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
-  </si>
-  <si>
-    <t>smtpServer</t>
-  </si>
-  <si>
-    <t>smtp.uq.edu.au</t>
-  </si>
-  <si>
-    <t>smtpPort</t>
-  </si>
-  <si>
-    <t>rpa.ads@its.uq.edu.au</t>
-  </si>
-  <si>
     <t>IAA_Vevo_ImmiAccount</t>
   </si>
   <si>
-    <t>IAA_Vevo_BusinessNotificationList</t>
-  </si>
-  <si>
-    <t>Text_BusinessNotificationList</t>
-  </si>
-  <si>
-    <t>Business users distribution list to be notified in case of application error during Sign In process</t>
-  </si>
-  <si>
-    <t>EmailSenderName</t>
-  </si>
-  <si>
-    <t>EmailFrom</t>
-  </si>
-  <si>
-    <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
+    <t>SignInError</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -501,6 +504,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -835,7 +841,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -847,7 +853,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
@@ -859,10 +865,10 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,10 +876,10 @@
         <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -881,10 +887,10 @@
         <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,82 +898,82 @@
         <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B20" s="9">
         <v>587</v>
@@ -1967,10 +1973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2067,7 +2073,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2200,93 +2206,110 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>82</v>
       </c>
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B33" t="s">
         <v>83</v>
       </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
-    </row>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" t="s">
-        <v>103</v>
-      </c>
-    </row>
+      <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3234,12 +3257,6 @@
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3251,7 +3268,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3297,36 +3314,30 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4332,7 +4343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4352,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>3</v>
@@ -4360,19 +4371,19 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -4382,16 +4393,16 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
@@ -4403,91 +4414,91 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C19" s="2"/>
     </row>

</xml_diff>

<commit_message>
ITSADSSD-17656 - Validate vevo case ref count in orchestrator queue
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -87,24 +87,6 @@
     <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
   </si>
   <si>
-    <t>AccuracyLow</t>
-  </si>
-  <si>
-    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyMedium</t>
-  </si>
-  <si>
-    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyHigh</t>
-  </si>
-  <si>
-    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
@@ -276,9 +258,6 @@
     <t>C:\Users\{0}\Downloads</t>
   </si>
   <si>
-    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
-  </si>
-  <si>
     <t>File name pattern for all document retrived from Immi website</t>
   </si>
   <si>
@@ -357,36 +336,9 @@
     <t>SystemException_CRM</t>
   </si>
   <si>
-    <t>ImmiErrorVevoInput</t>
-  </si>
-  <si>
-    <t>An exception occurred while entering Vevo details on Immi website</t>
-  </si>
-  <si>
-    <t>ImmiErrorDownloadSearchResult</t>
-  </si>
-  <si>
-    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
-  </si>
-  <si>
-    <t>smtpServer</t>
-  </si>
-  <si>
-    <t>smtp.uq.edu.au</t>
-  </si>
-  <si>
-    <t>smtpPort</t>
-  </si>
-  <si>
     <t>rpa.ads@its.uq.edu.au</t>
   </si>
   <si>
-    <t>EmailSenderName</t>
-  </si>
-  <si>
-    <t>EmailFrom</t>
-  </si>
-  <si>
     <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
   </si>
   <si>
@@ -427,6 +379,112 @@
   </si>
   <si>
     <t>SignInError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix for Immi website search result in case no pdf found </t>
+  </si>
+  <si>
+    <t>Victor (RPA) has successfully checked the Visa details and has attached a PDF of the results to this ticket.</t>
+  </si>
+  <si>
+    <t>VevoSearch_Success</t>
+  </si>
+  <si>
+    <t>VevoSearch_NoResult</t>
+  </si>
+  <si>
+    <t>VevoMaxCountExceed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to unexpected system error this vevo check could not be completed Victor (RPA). The RPA team have been automatically notified of the error.
+</t>
+  </si>
+  <si>
+    <t>Victor (RPA) attempted to check the Visa details but received an error. Please check that all of the details provided are correct. A screenshot of the error has been attached to this ticket.</t>
+  </si>
+  <si>
+    <t>GetVevoDetailsException</t>
+  </si>
+  <si>
+    <t>ImmiSearchException</t>
+  </si>
+  <si>
+    <t>UploadImmiResultException</t>
+  </si>
+  <si>
+    <t>AssignToVevoCheckOutCategoryException</t>
+  </si>
+  <si>
+    <t>An error occurred while assigning case reference to Vevo Check Out category in Oracle CRM.</t>
+  </si>
+  <si>
+    <t>SaveAndCloseException</t>
+  </si>
+  <si>
+    <t>An error occurred while trying to save and close the case reference on Oracle CRM.</t>
+  </si>
+  <si>
+    <t>An error occurred while writing Vevo search result note in Oracle CRM.</t>
+  </si>
+  <si>
+    <t>WriteVevoResultException</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName</t>
+  </si>
+  <si>
+    <t>SenderEmailID</t>
+  </si>
+  <si>
+    <t>Victor - RPA Bot</t>
+  </si>
+  <si>
+    <t>noreply@uq.edu.au</t>
+  </si>
+  <si>
+    <t>IAA_Vevo_BusinessNotificationList</t>
+  </si>
+  <si>
+    <t>Business user distribution list for Vevo Check process</t>
+  </si>
+  <si>
+    <t>BusinessNotificationList</t>
+  </si>
+  <si>
+    <t>VevoMaxRetryCount</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>SMTP_PORT</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>UQ internal SMTP Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ internal SMTP Server Port number </t>
+  </si>
+  <si>
+    <t>An error occurred while retrieving Vevo details from Oracle CRM.</t>
+  </si>
+  <si>
+    <t>An error occurred while performing Vevo search on Immi website.</t>
+  </si>
+  <si>
+    <t>An error occurred while uploading Vevo search on Oracle CRM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category with performing any action. Please check the system logs and ensure if this is one of the occurrence. The case reference is :  </t>
+  </si>
+  <si>
+    <t>VevoMaxCountExceedEmailErrorMsg</t>
   </si>
 </sst>
 </file>
@@ -493,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -506,6 +564,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -790,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -838,159 +899,149 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="9">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1973,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2118,198 +2169,181 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>0.6</v>
+      <c r="B15" t="s">
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>0.8</v>
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17">
-        <v>0.9</v>
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-    </row>
+        <v>142</v>
+      </c>
+      <c r="B27" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>82</v>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3253,13 +3287,12 @@
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3268,7 +3301,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3314,33 +3347,59 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4341,10 +4400,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4363,27 +4422,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -4393,16 +4450,16 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
@@ -4414,93 +4471,157 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to Get transaction, exception messages and email template
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>https://uqapplications.crm.test.uq.edu.au/AgentWeb/</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
     <t>UQ Oracle CRM  URL for Dev environment</t>
   </si>
   <si>
@@ -264,12 +261,6 @@
     <t>File path for all document retrived from Immi website</t>
   </si>
   <si>
-    <t>Config Not Initialised</t>
-  </si>
-  <si>
-    <t>Mode Asset Missing</t>
-  </si>
-  <si>
     <t>Extras</t>
   </si>
   <si>
@@ -321,27 +312,9 @@
     <t>DoB_Label_Missing</t>
   </si>
   <si>
-    <t>Couldn't find my operation mode asset at OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>Couldn't get my settings from the config: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An unexpected error occurred in CRM: </t>
-  </si>
-  <si>
-    <t>SystemException_Immi</t>
-  </si>
-  <si>
-    <t>SystemException_CRM</t>
-  </si>
-  <si>
     <t>rpa.ads@its.uq.edu.au</t>
   </si>
   <si>
-    <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
-  </si>
-  <si>
     <t>Victor's (RPA bot for Vevo check) Immi account login  (Type: Credential)</t>
   </si>
   <si>
@@ -385,12 +358,6 @@
   </si>
   <si>
     <t>Victor (RPA) has successfully checked the Visa details and has attached a PDF of the results to this ticket.</t>
-  </si>
-  <si>
-    <t>VevoSearch_Success</t>
-  </si>
-  <si>
-    <t>VevoSearch_NoResult</t>
   </si>
   <si>
     <t>VevoMaxCountExceed</t>
@@ -457,12 +424,6 @@
     <t>UQ_SMTP_SERVER</t>
   </si>
   <si>
-    <t>SMTP_SERVER</t>
-  </si>
-  <si>
-    <t>SMTP_PORT</t>
-  </si>
-  <si>
     <t>UQ_SMTP_PORT</t>
   </si>
   <si>
@@ -481,10 +442,40 @@
     <t>An error occurred while uploading Vevo search on Oracle CRM.</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category with performing any action. Please check the system logs and ensure if this is one of the occurrence. The case reference is :  </t>
-  </si>
-  <si>
     <t>VevoMaxCountExceedEmailErrorMsg</t>
+  </si>
+  <si>
+    <t>VevoSearch_Success_LogMsg</t>
+  </si>
+  <si>
+    <t>VevoSearch_NoResult_LogMsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEVO Visa Details Check successful and pdf found for Case Reference : </t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check returned No Result for Case Reference :</t>
+  </si>
+  <si>
+    <t>VevoSearch_Success_CRM_Note</t>
+  </si>
+  <si>
+    <t>VevoSearch_NoResult_CRM_Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category with performing any action. Please check the system logs and ensure if this is one of the occurrence? The case reference is :  </t>
+  </si>
+  <si>
+    <t>VevoInitErrorEmailMsg</t>
+  </si>
+  <si>
+    <t>You are receiving this email from RPA Robot due to an error encountred in Vevo Check process during initialisation. Please see attached screen shot.</t>
+  </si>
+  <si>
+    <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
+  </si>
+  <si>
+    <t>*********TBC*********</t>
   </si>
 </sst>
 </file>
@@ -551,15 +542,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -851,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -902,7 +891,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -914,7 +903,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -926,10 +915,10 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -940,7 +929,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -951,18 +940,18 @@
         <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
+      <c r="B9" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -971,64 +960,64 @@
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
         <v>56</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
         <v>58</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2010,13 +1999,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B11" r:id="rId3"/>
-    <hyperlink ref="B13" r:id="rId4"/>
-    <hyperlink ref="B14" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B16" r:id="rId7"/>
-    <hyperlink ref="B15" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B16" r:id="rId6"/>
+    <hyperlink ref="B15" r:id="rId7"/>
+    <hyperlink ref="B6" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2124,7 +2113,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2224,110 +2213,110 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="11">
+        <v>131</v>
+      </c>
+      <c r="B27" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
         <v>76</v>
       </c>
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3301,7 +3290,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3347,57 +3336,57 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4400,10 +4389,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4422,56 +4411,62 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>148</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -4482,145 +4477,123 @@
         <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
+      <c r="A14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
+      <c r="A15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" t="s">
         <v>121</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for NoItemToProcess, error logging and reporting
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="155">
   <si>
     <t>Name</t>
   </si>
@@ -340,12 +340,6 @@
   </si>
   <si>
     <t>https://online.immi.gov.au/lusc/login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
-  </si>
-  <si>
-    <t>SSO_rpa00001</t>
   </si>
   <si>
     <t>IAA_Vevo_ImmiAccount</t>
@@ -463,9 +457,6 @@
     <t>VevoSearch_NoResult_CRM_Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category with performing any action. Please check the system logs and ensure if this is one of the occurrence? The case reference is :  </t>
-  </si>
-  <si>
     <t>VevoInitErrorEmailMsg</t>
   </si>
   <si>
@@ -476,6 +467,27 @@
   </si>
   <si>
     <t>*********TBC*********</t>
+  </si>
+  <si>
+    <t>Maximum number of re-try attempts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
+  </si>
+  <si>
+    <t>SSO_rpa00001</t>
+  </si>
+  <si>
+    <t>VevoSearch_Success</t>
+  </si>
+  <si>
+    <t>VevoSearch_NoResult</t>
+  </si>
+  <si>
+    <t>manish.gupta@uq.edu.au;s.gururaj@uq.edu.au;shyni.joseph@uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -841,7 +853,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -915,7 +927,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
@@ -948,7 +960,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>49</v>
@@ -983,7 +995,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -2013,10 +2025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2264,7 @@
         <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,59 +2280,76 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" t="s">
-        <v>109</v>
-      </c>
-    </row>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>81</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" t="s">
         <v>124</v>
       </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3276,9 +3305,11 @@
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1"/>
+    <hyperlink ref="B36" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3290,7 +3321,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3339,10 +3370,10 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3350,7 +3381,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>97</v>
@@ -3358,35 +3389,35 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4392,7 +4423,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4417,10 +4448,10 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -4498,102 +4529,102 @@
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Config change for test email distribution list
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -485,9 +485,6 @@
   </si>
   <si>
     <t>VevoSearch_NoResult</t>
-  </si>
-  <si>
-    <t>manish.gupta@uq.edu.au;s.gururaj@uq.edu.au;shyni.joseph@uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -853,7 +850,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -995,7 +992,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
BRE for Country of document not available in ImmiAccount
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>VevoSearch_NoResult</t>
+  </si>
+  <si>
+    <t>Country_NotFound</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. 'Country of Document' value does not match any options on the ImmiAccount website - please check that a valid value has been provided.</t>
   </si>
 </sst>
 </file>
@@ -849,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2025,7 +2031,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4417,10 +4423,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4524,103 +4530,111 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="2"/>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>110</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>137</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>114</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>115</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>121</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>116</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change email distribution list to ITS RPA for TEST environment
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -2016,11 +2016,11 @@
     <hyperlink ref="B7" r:id="rId1"/>
     <hyperlink ref="B11" r:id="rId2"/>
     <hyperlink ref="B13" r:id="rId3"/>
-    <hyperlink ref="B14" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B16" r:id="rId6"/>
-    <hyperlink ref="B15" r:id="rId7"/>
-    <hyperlink ref="B6" r:id="rId8"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B16" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
+    <hyperlink ref="B14" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4425,7 +4425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Config changes in config.xlsx
Added CRM production URL and remove version number from queue name. Both changes in config.xlsx only no code changes
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>https://uqapplications.crm.test.uq.edu.au/AgentWeb/</t>
   </si>
   <si>
-    <t>UQ Oracle CRM  URL for Dev environment</t>
-  </si>
-  <si>
     <t>UQ Oracle CRM  URL for Test environment</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>IAA_VevoCheck</t>
-  </si>
-  <si>
-    <t>IAA_VevoCheck-1.0</t>
   </si>
   <si>
     <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
@@ -463,34 +457,55 @@
     <t>You are receiving this email from RPA Robot due to an error encountred in Vevo Check process during initialisation. Please see attached screen shot.</t>
   </si>
   <si>
+    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
+  </si>
+  <si>
+    <t>SSO_rpa00001</t>
+  </si>
+  <si>
+    <t>VevoSearch_Success</t>
+  </si>
+  <si>
+    <t>VevoSearch_NoResult</t>
+  </si>
+  <si>
+    <t>Country_NotFound</t>
+  </si>
+  <si>
+    <t>RPA could not complete this Vevo check. 'Country of Document' value does not match any options on the ImmiAccount website - please check that a valid value has been provided.</t>
+  </si>
+  <si>
+    <t>https://support.future-students.uq.edu.au/AgentWeb</t>
+  </si>
+  <si>
+    <t>UQ Oracle CRM  URL for Dev environment</t>
+  </si>
+  <si>
     <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
   </si>
   <si>
-    <t>*********TBC*********</t>
-  </si>
-  <si>
-    <t>Maximum number of re-try attempts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
-  </si>
-  <si>
-    <t>SSO_rpa00001</t>
-  </si>
-  <si>
-    <t>VevoSearch_Success</t>
-  </si>
-  <si>
-    <t>VevoSearch_NoResult</t>
-  </si>
-  <si>
-    <t>Country_NotFound</t>
-  </si>
-  <si>
-    <t>RPA could not complete this Vevo check. 'Country of Document' value does not match any options on the ImmiAccount website - please check that a valid value has been provided.</t>
+    <t>Reporting tag if visa details found on Immi website</t>
+  </si>
+  <si>
+    <t>Reporting tag if no visa details found on Immi website</t>
+  </si>
+  <si>
+    <t>Tag value to indicate error occurred during sign in and send email to business user (in Production )</t>
+  </si>
+  <si>
+    <t>Constant for Oracle CRM base URL. This value appended with operating environment and retrive CRM URL from settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vevo bot display name for email notifications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vevo bot sender email (for display purpose) email sent through SMTP </t>
+  </si>
+  <si>
+    <t>Maximum number of re-try attempts for successive application errors</t>
   </si>
 </sst>
 </file>
@@ -855,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -906,7 +921,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -918,7 +933,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -930,10 +945,10 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -944,7 +959,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,7 +970,7 @@
         <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -963,10 +978,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -975,55 +990,55 @@
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
         <v>57</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2019,8 +2034,9 @@
     <hyperlink ref="B8" r:id="rId4"/>
     <hyperlink ref="B16" r:id="rId5"/>
     <hyperlink ref="B15" r:id="rId6"/>
-    <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B14" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2030,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2128,7 +2144,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2228,143 +2244,161 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s">
-        <v>100</v>
-      </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" s="9">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+      <c r="C29" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
         <v>76</v>
-      </c>
-      <c r="C31" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3370,57 +3404,57 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4445,197 +4479,197 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Config change only -  CRM prod URL
Change CRM production URL to https://uqapplications.custhelp.com/AgentWeb as confirmed by Steve (CRM team). No code changes
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -478,9 +478,6 @@
     <t>RPA could not complete this Vevo check. 'Country of Document' value does not match any options on the ImmiAccount website - please check that a valid value has been provided.</t>
   </si>
   <si>
-    <t>https://support.future-students.uq.edu.au/AgentWeb</t>
-  </si>
-  <si>
     <t>UQ Oracle CRM  URL for Dev environment</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>Maximum number of re-try attempts for successive application errors</t>
+  </si>
+  <si>
+    <t>https://uqapplications.custhelp.com/AgentWeb</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -945,10 +945,10 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>48</v>
@@ -2046,7 +2046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2305,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
         <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
         <v>148</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2350,7 @@
         <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2373,7 @@
         <v>122</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-18779 - IELTS website automation
Initial commit for login into IELTS website and navigate to TRF Query section
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -464,9 +464,6 @@
   </si>
   <si>
     <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
-  </si>
-  <si>
-    <t>*********TBC*********</t>
   </si>
   <si>
     <t>Maximum number of re-try attempts.</t>
@@ -853,7 +850,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -959,9 +956,7 @@
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
@@ -995,7 +990,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -2286,23 +2281,23 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3370,10 +3365,10 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4576,7 +4571,7 @@
         <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ITSADSSD-19478 - IAA_VevoCheck Change
Amend package description, email sender name, subject and message, increase timeout to 90 seconds, add log entry to indicate transaction end
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -454,9 +454,6 @@
     <t>VevoInitErrorEmailMsg</t>
   </si>
   <si>
-    <t>You are receiving this email from RPA Robot due to an error encountred in Vevo Check process during initialisation. Please see attached screen shot.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
   </si>
   <si>
@@ -481,31 +478,55 @@
     <t>UQ Oracle CRM  URL for Dev environment</t>
   </si>
   <si>
+    <t>Reporting tag if visa details found on Immi website</t>
+  </si>
+  <si>
+    <t>Reporting tag if no visa details found on Immi website</t>
+  </si>
+  <si>
+    <t>Tag value to indicate error occurred during sign in and send email to business user (in Production )</t>
+  </si>
+  <si>
+    <t>Constant for Oracle CRM base URL. This value appended with operating environment and retrive CRM URL from settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vevo bot display name for email notifications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vevo bot sender email (for display purpose) email sent through SMTP </t>
+  </si>
+  <si>
+    <t>Maximum number of re-try attempts for successive application errors</t>
+  </si>
+  <si>
+    <t>https://uqapplications.custhelp.com/AgentWeb</t>
+  </si>
+  <si>
+    <t>PROD_Subject</t>
+  </si>
+  <si>
+    <t>NonPROD_Subject</t>
+  </si>
+  <si>
+    <t>You are receiving this email from the RPA robot due to an error encountered during the Vevo Check sign-in process. Please see attached screenshot.</t>
+  </si>
+  <si>
+    <t>Victor found error(s) while processing</t>
+  </si>
+  <si>
+    <t>Victor {0} found error(s) while processing</t>
+  </si>
+  <si>
+    <t>Vevo bot display name for email notifications for Non Prod environments (Dev/Test/Staging)</t>
+  </si>
+  <si>
+    <t>Victor {0} - RPA Bot</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName_NP</t>
+  </si>
+  <si>
     <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
-  </si>
-  <si>
-    <t>Reporting tag if visa details found on Immi website</t>
-  </si>
-  <si>
-    <t>Reporting tag if no visa details found on Immi website</t>
-  </si>
-  <si>
-    <t>Tag value to indicate error occurred during sign in and send email to business user (in Production )</t>
-  </si>
-  <si>
-    <t>Constant for Oracle CRM base URL. This value appended with operating environment and retrive CRM URL from settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vevo bot display name for email notifications </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vevo bot sender email (for display purpose) email sent through SMTP </t>
-  </si>
-  <si>
-    <t>Maximum number of re-try attempts for successive application errors</t>
-  </si>
-  <si>
-    <t>https://uqapplications.custhelp.com/AgentWeb</t>
   </si>
 </sst>
 </file>
@@ -871,7 +892,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -945,10 +966,10 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,7 +999,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>48</v>
@@ -2044,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2305,29 +2326,29 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2371,7 @@
         <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2361,7 +2382,7 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2373,21 +2394,31 @@
         <v>122</v>
       </c>
       <c r="C35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C36" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C37" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3344,9 +3375,10 @@
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1"/>
+    <hyperlink ref="B37" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3407,10 +3439,10 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4457,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4488,7 +4520,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -4566,10 +4598,10 @@
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" t="s">
         <v>149</v>
-      </c>
-      <c r="B12" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4621,54 +4653,70 @@
         <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>132</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>116</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ITSADSSD-19935 - IAA_VevoCheck - Junk character bug fix
Regular expression to whitelist, remove junk character &nbsp,  Close dashboard prior to logout to handle leave site pop up and set time out for invokeCloseApplication workflow
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -526,7 +526,7 @@
     <t>EmailSenderDisplayName_NP</t>
   </si>
   <si>
-    <t>https://uqapplications--tst1.custhelp.com/AgentWeb/</t>
+    <t>RegEx_Error</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -966,7 +966,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>150</v>
@@ -4489,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -4650,73 +4650,81 @@
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>160</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>116</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ITSADSSD-19935 - IAA_VevoCheck  v1.1 - DoB format message and BRE for regex
DoB format message and BRE for regex return no result
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>RegEx_Error</t>
+  </si>
+  <si>
+    <t>VevoRegExParseErrorEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - RegularExpressionError. Victor unable to parse Vevo check input details. Case reference is : </t>
   </si>
 </sst>
 </file>
@@ -891,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2067,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4489,10 +4495,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4650,81 +4656,89 @@
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>160</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ITSADSSD-20744 - IAA_VevoCheck v1.1
Add Find element to ensure case ref is visible, RegEx to handle multiple spaces and closeAllApplication
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -370,9 +370,6 @@
     <t>AssignToVevoCheckOutCategoryException</t>
   </si>
   <si>
-    <t>An error occurred while assigning case reference to Vevo Check Out category in Oracle CRM.</t>
-  </si>
-  <si>
     <t>SaveAndCloseException</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>VevoInitErrorEmailMsg</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Victor's (RPA bot for Vevo check) Single Sign On account 'RPA00001'  (Type: Credential) </t>
   </si>
   <si>
@@ -533,6 +527,12 @@
   </si>
   <si>
     <t xml:space="preserve">Attention - RegularExpressionError. Victor unable to parse Vevo check input details. Case reference is : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - VevoMaxRetryCount exceeded. Victor assigning this case to Vevo Check Out category without performing any checks on Immi website. Please check the system logs and ensure if this is one of the occurrences? Case reference is :  </t>
+  </si>
+  <si>
+    <t>An error occurred while assigning case to Vevo Check Out category in Oracle CRM.</t>
   </si>
 </sst>
 </file>
@@ -576,6 +576,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -975,7 +976,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1005,7 +1006,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>48</v>
@@ -2073,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2125,7 +2126,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2326,35 +2327,35 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="9">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2377,7 +2378,7 @@
         <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2388,41 +2389,41 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3445,10 +3446,10 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3464,35 +3465,35 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4497,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4523,10 +4524,10 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -4604,15 +4605,15 @@
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>107</v>
@@ -4621,7 +4622,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>110</v>
@@ -4630,25 +4631,25 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -4656,10 +4657,10 @@
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4672,26 +4673,26 @@
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" t="s">
-        <v>143</v>
+        <v>134</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4699,7 +4700,7 @@
         <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4707,7 +4708,7 @@
         <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4715,15 +4716,15 @@
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4731,15 +4732,15 @@
         <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
         <v>116</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>